<commit_message>
Fixing bug in plug.
</commit_message>
<xml_diff>
--- a/example/info/01 prepared info.xlsx
+++ b/example/info/01 prepared info.xlsx
@@ -436,17 +436,17 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>test id</t>
+          <t>test_id</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>old filename</t>
+          <t>old_filename</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>test type</t>
+          <t>test_type</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -471,12 +471,12 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>A_0 (mm)</t>
+          <t>A_0_(mm)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>h_0 (mm)</t>
+          <t>h_0_(mm)</t>
         </is>
       </c>
     </row>

</xml_diff>